<commit_message>
experimental data 1 classification
</commit_message>
<xml_diff>
--- a/data/olhs_run1.xlsx
+++ b/data/olhs_run1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="592" documentId="13_ncr:1_{86A97CFE-042D-E84B-9B3A-A2422876EAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{480108D6-99C7-42C7-B4DB-9A60E01013F6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2E69A4AB-BA25-3440-870D-57BCBE9E2EF8}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19660" activeTab="1" xr2:uid="{2E69A4AB-BA25-3440-870D-57BCBE9E2EF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Design (OLHS)" sheetId="1" r:id="rId1"/>
@@ -300,10 +300,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -341,7 +345,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -447,7 +451,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -589,7 +593,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -606,19 +610,19 @@
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="42.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -637,7 +641,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -666,7 +670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -695,7 +699,7 @@
         <v>82.631578947368396</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f>A3+1</f>
         <v>2</v>
@@ -725,7 +729,7 @@
         <v>74.736842105263193</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A22" si="0">A4+1</f>
         <v>3</v>
@@ -755,7 +759,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -785,7 +789,7 @@
         <v>77.894736842105303</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -815,7 +819,7 @@
         <v>92.105263157894697</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -845,7 +849,7 @@
         <v>84.210526315789494</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -875,7 +879,7 @@
         <v>71.578947368421098</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -905,7 +909,7 @@
         <v>81.052631578947398</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -935,7 +939,7 @@
         <v>73.157894736842096</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -965,7 +969,7 @@
         <v>98.421052631579002</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -995,7 +999,7 @@
         <v>79.473684210526301</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1025,7 +1029,7 @@
         <v>85.789473684210506</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1055,7 +1059,7 @@
         <v>76.315789473684205</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1085,7 +1089,7 @@
         <v>87.368421052631604</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1115,7 +1119,7 @@
         <v>93.684210526315795</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1145,7 +1149,7 @@
         <v>95.263157894736906</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1175,7 +1179,7 @@
         <v>96.842105263157904</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1205,7 +1209,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1235,7 +1239,7 @@
         <v>88.947368421052602</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="19" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1279,24 +1283,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498369C7-30ED-4465-89FD-A4CA38E6109C}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.75" customWidth="1"/>
-    <col min="11" max="13" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" customWidth="1"/>
+    <col min="11" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1338,7 +1342,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1380,7 +1384,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1423,7 +1427,7 @@
         <v>67.91</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -1465,7 +1469,7 @@
         <v>53.62</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -1507,7 +1511,7 @@
         <v>78.95</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -1549,7 +1553,7 @@
         <v>85.62</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -1592,7 +1596,7 @@
         <v>8.6300000000000008</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -1634,7 +1638,7 @@
         <v>56.85</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1677,7 +1681,7 @@
         <v>10.68</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1719,7 +1723,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -1761,7 +1765,7 @@
         <v>80.45</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -1803,7 +1807,7 @@
         <v>79.38</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -1846,7 +1850,7 @@
         <v>74.91</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -1889,7 +1893,7 @@
         <v>67.790000000000006</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -1931,7 +1935,7 @@
         <v>35.840000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -1973,7 +1977,7 @@
         <v>85.79</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -2015,7 +2019,7 @@
         <v>73.05</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -2057,7 +2061,7 @@
         <v>81.61</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -2100,7 +2104,7 @@
         <v>82.15</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -2142,7 +2146,7 @@
         <v>35.53</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -2184,7 +2188,7 @@
         <v>-7.8</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -2226,7 +2230,7 @@
         <v>70.650000000000006</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2235,7 +2239,7 @@
       </c>
       <c r="C24" s="16"/>
     </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>14</v>
       </c>
@@ -2244,7 +2248,7 @@
       </c>
       <c r="C25" s="14"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
data olhs run 1
</commit_message>
<xml_diff>
--- a/data/olhs_run1.xlsx
+++ b/data/olhs_run1.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nuwildcat-my.sharepoint.com/personal/rmj4546_ads_northwestern_edu/Documents/Documents/NU/Projects/sprayableHydrogel_GT/sprayable-hydrogels/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="592" documentId="13_ncr:1_{86A97CFE-042D-E84B-9B3A-A2422876EAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{480108D6-99C7-42C7-B4DB-9A60E01013F6}"/>
+  <xr:revisionPtr revIDLastSave="615" documentId="13_ncr:1_{86A97CFE-042D-E84B-9B3A-A2422876EAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C06D3175-A46C-458F-B3C0-CD70EBC1643F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19660" activeTab="1" xr2:uid="{2E69A4AB-BA25-3440-870D-57BCBE9E2EF8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2E69A4AB-BA25-3440-870D-57BCBE9E2EF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Design (OLHS)" sheetId="1" r:id="rId1"/>
     <sheet name="data" sheetId="3" r:id="rId2"/>
+    <sheet name="feasibility" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
   <si>
     <t>Block Size</t>
   </si>
@@ -305,9 +306,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -345,7 +346,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -451,7 +452,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -593,7 +594,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -607,22 +608,22 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection sqref="A1:I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="42.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -641,7 +642,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -670,7 +671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -699,7 +700,7 @@
         <v>82.631578947368396</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>A3+1</f>
         <v>2</v>
@@ -729,7 +730,7 @@
         <v>74.736842105263193</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A22" si="0">A4+1</f>
         <v>3</v>
@@ -759,7 +760,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -789,7 +790,7 @@
         <v>77.894736842105303</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -819,7 +820,7 @@
         <v>92.105263157894697</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -849,7 +850,7 @@
         <v>84.210526315789494</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -879,7 +880,7 @@
         <v>71.578947368421098</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -909,7 +910,7 @@
         <v>81.052631578947398</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -939,7 +940,7 @@
         <v>73.157894736842096</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -969,7 +970,7 @@
         <v>98.421052631579002</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -999,7 +1000,7 @@
         <v>79.473684210526301</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1029,7 +1030,7 @@
         <v>85.789473684210506</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1059,7 +1060,7 @@
         <v>76.315789473684205</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1089,7 +1090,7 @@
         <v>87.368421052631604</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1119,7 +1120,7 @@
         <v>93.684210526315795</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1149,7 +1150,7 @@
         <v>95.263157894736906</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1179,7 +1180,7 @@
         <v>96.842105263157904</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1209,7 +1210,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1239,7 +1240,7 @@
         <v>88.947368421052602</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1283,24 +1284,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498369C7-30ED-4465-89FD-A4CA38E6109C}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.625" customWidth="1"/>
+    <col min="11" max="13" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>11</v>
       </c>
@@ -1342,7 +1343,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1384,7 +1385,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1427,7 +1428,7 @@
         <v>67.91</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -1469,7 +1470,7 @@
         <v>53.62</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -1511,7 +1512,7 @@
         <v>78.95</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -1553,7 +1554,7 @@
         <v>85.62</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -1596,7 +1597,7 @@
         <v>8.6300000000000008</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -1638,7 +1639,7 @@
         <v>56.85</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1681,7 +1682,7 @@
         <v>10.68</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1723,7 +1724,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -1765,7 +1766,7 @@
         <v>80.45</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -1807,7 +1808,7 @@
         <v>79.38</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -1850,7 +1851,7 @@
         <v>74.91</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -1893,7 +1894,7 @@
         <v>67.790000000000006</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -1935,7 +1936,7 @@
         <v>35.840000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -1977,7 +1978,7 @@
         <v>85.79</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -2019,7 +2020,7 @@
         <v>73.05</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -2061,7 +2062,7 @@
         <v>81.61</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -2104,7 +2105,7 @@
         <v>82.15</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -2146,7 +2147,7 @@
         <v>35.53</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -2188,7 +2189,7 @@
         <v>-7.8</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -2230,7 +2231,7 @@
         <v>70.650000000000006</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2239,7 +2240,7 @@
       </c>
       <c r="C24" s="16"/>
     </row>
-    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>14</v>
       </c>
@@ -2248,7 +2249,7 @@
       </c>
       <c r="C25" s="14"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>13</v>
       </c>
@@ -2263,4 +2264,132 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F9ED10A-C07B-4A8B-B026-E834F398AC15}">
+  <dimension ref="A1:A22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>